<commit_message>
Updated Frontend, layouts, added tests
</commit_message>
<xml_diff>
--- a/esc project template _fixed.xlsx
+++ b/esc project template _fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESC Project\FrontEnd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A7D190-9BEE-4FC7-B02E-3B857806B436}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18704E25-BF30-471F-AF88-C8202BA6B2DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11385" xr2:uid="{3C774843-307A-40CD-85CD-B70ACD0E23E3}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{3C774843-307A-40CD-85CD-B70ACD0E23E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="76">
   <si>
     <t>Project Name</t>
   </si>
@@ -202,6 +202,63 @@
   </si>
   <si>
     <t>Proj E05 - IOT</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>S07</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>S08</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>E03</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>E01</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>S09</t>
+  </si>
+  <si>
+    <t>S01</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>P47</t>
+  </si>
+  <si>
+    <t>E02</t>
+  </si>
+  <si>
+    <t>E05</t>
   </si>
 </sst>
 </file>
@@ -237,10 +294,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +616,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +664,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -631,8 +689,8 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -660,8 +718,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -690,7 +748,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -719,7 +777,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
@@ -747,8 +805,8 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+      <c r="A7" t="s">
+        <v>59</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -773,8 +831,8 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
+      <c r="A8" t="s">
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -800,7 +858,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -852,7 +910,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -877,8 +935,8 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
+      <c r="A12" t="s">
+        <v>61</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -904,7 +962,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -930,7 +988,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -955,8 +1013,8 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
+      <c r="A15" t="s">
+        <v>62</v>
       </c>
       <c r="B15" t="s">
         <v>26</v>
@@ -981,8 +1039,8 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
+      <c r="A16" t="s">
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
@@ -1007,8 +1065,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
+      <c r="A17" t="s">
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -1033,8 +1091,8 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
+      <c r="A18" t="s">
+        <v>65</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
@@ -1059,8 +1117,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
+      <c r="A19" t="s">
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -1085,8 +1143,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
+      <c r="A20" t="s">
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -1112,7 +1170,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
@@ -1137,6 +1195,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>24</v>
+      </c>
       <c r="B22" t="s">
         <v>33</v>
       </c>
@@ -1157,6 +1218,9 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>11</v>
+      </c>
       <c r="B23" t="s">
         <v>34</v>
       </c>
@@ -1177,6 +1241,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>59</v>
+      </c>
       <c r="B24" t="s">
         <v>35</v>
       </c>
@@ -1197,6 +1264,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="B25" t="s">
         <v>36</v>
       </c>
@@ -1217,6 +1287,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>68</v>
+      </c>
       <c r="B26" t="s">
         <v>37</v>
       </c>
@@ -1237,6 +1310,9 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7</v>
+      </c>
       <c r="B27" t="s">
         <v>38</v>
       </c>
@@ -1257,6 +1333,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>32</v>
+      </c>
       <c r="B28" t="s">
         <v>39</v>
       </c>
@@ -1277,6 +1356,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
       <c r="B29" t="s">
         <v>40</v>
       </c>
@@ -1297,6 +1379,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>43</v>
+      </c>
       <c r="B30" t="s">
         <v>41</v>
       </c>
@@ -1317,6 +1402,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>17</v>
+      </c>
       <c r="B31" t="s">
         <v>42</v>
       </c>
@@ -1337,6 +1425,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>45</v>
+      </c>
       <c r="B32" t="s">
         <v>43</v>
       </c>
@@ -1356,7 +1447,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>50</v>
+      </c>
       <c r="B33" t="s">
         <v>44</v>
       </c>
@@ -1376,7 +1470,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>10</v>
+      </c>
       <c r="B34" t="s">
         <v>45</v>
       </c>
@@ -1396,7 +1493,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>13</v>
+      </c>
       <c r="B35" t="s">
         <v>46</v>
       </c>
@@ -1416,7 +1516,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
       <c r="B36" t="s">
         <v>47</v>
       </c>
@@ -1436,7 +1539,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>71</v>
+      </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
@@ -1456,7 +1562,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>46</v>
+      </c>
       <c r="B38" t="s">
         <v>49</v>
       </c>
@@ -1476,7 +1585,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>72</v>
+      </c>
       <c r="B39" t="s">
         <v>50</v>
       </c>
@@ -1496,7 +1608,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>44</v>
+      </c>
       <c r="B40" t="s">
         <v>51</v>
       </c>
@@ -1516,7 +1631,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>21</v>
+      </c>
       <c r="B41" t="s">
         <v>52</v>
       </c>
@@ -1536,7 +1654,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>73</v>
+      </c>
       <c r="B42" t="s">
         <v>53</v>
       </c>
@@ -1556,7 +1677,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>74</v>
+      </c>
       <c r="B43" t="s">
         <v>54</v>
       </c>
@@ -1576,7 +1700,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>15</v>
+      </c>
       <c r="B44" t="s">
         <v>55</v>
       </c>
@@ -1596,7 +1723,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
       <c r="B45" t="s">
         <v>56</v>
       </c>

</xml_diff>